<commit_message>
Refactor ExcelToMySQL: - Insert/Update logic corrected - Added unique key check, now shows 'Done deja egziste' instead of duplicate error - Logs updated with insert, exists, error types - Removed old mapping issues causing undefined columns - Frontend JS ready to display logs with filters and progress - Prepared process.php to reset form and handle modal messages
</commit_message>
<xml_diff>
--- a/public/uploads/data.xlsx
+++ b/public/uploads/data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Nom</t>
   </si>
@@ -32,6 +32,18 @@
   </si>
   <si>
     <t>jonatha@icloud.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joberno </t>
+  </si>
+  <si>
+    <t>j@gmail.com</t>
+  </si>
+  <si>
+    <t>ahsah</t>
+  </si>
+  <si>
+    <t>asdasd@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -325,8 +337,28 @@
         <v>40.0</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1"/>
-    <row r="5" ht="14.25" customHeight="1"/>
+    <row r="4" ht="14.25" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>40.0</v>
+      </c>
+    </row>
     <row r="6" ht="14.25" customHeight="1"/>
     <row r="7" ht="14.25" customHeight="1"/>
     <row r="8" ht="14.25" customHeight="1"/>

</xml_diff>